<commit_message>
Update a stateDescription of RaceOfPersonCode.
</commit_message>
<xml_diff>
--- a/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesHawaii.xlsx
+++ b/tools/nibrs-staging-data/src/test/resources/codeSpreadSheets/NIBRSCodeTablesHawaii.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27220" yWindow="8940" windowWidth="23280" windowHeight="12900" tabRatio="705" firstSheet="17" activeTab="18"/>
+    <workbookView xWindow="22980" yWindow="2820" windowWidth="20240" windowHeight="12160" tabRatio="705" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2292" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2292" uniqueCount="719">
   <si>
     <t>Table</t>
   </si>
@@ -2204,6 +2204,9 @@
   </si>
   <si>
     <t>Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>American Indian</t>
   </si>
 </sst>
 </file>
@@ -6513,7 +6516,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6581,7 +6584,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>388</v>
+        <v>718</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>35</v>

</xml_diff>